<commit_message>
modifications to person sheet done, please continue
Oliver, I sent you an email with comments.
</commit_message>
<xml_diff>
--- a/SRC/Research results sample - persons.xlsx
+++ b/SRC/Research results sample - persons.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mira\Dropbox\Lesewelten\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1856,7 +1851,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -1903,12 +1898,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1940,13 +1941,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2302,9 +2306,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -2325,7 +2329,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -2387,15 +2391,20 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
       <c r="Q2" t="s">
         <v>22</v>
       </c>
@@ -2410,15 +2419,18 @@
       </c>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" t="s">
         <v>29</v>
       </c>
@@ -2440,10 +2452,10 @@
       <c r="N3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="Q3" t="s">
@@ -2457,16 +2469,18 @@
       </c>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F4">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
         <v>1969</v>
       </c>
       <c r="G4" t="s">
@@ -2481,7 +2495,8 @@
       <c r="L4" t="s">
         <v>47</v>
       </c>
-      <c r="P4" t="s">
+      <c r="O4" s="5"/>
+      <c r="P4" s="5" t="s">
         <v>48</v>
       </c>
       <c r="Q4" t="s">
@@ -2501,22 +2516,26 @@
       </c>
     </row>
     <row r="5" spans="1:25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
         <v>56</v>
       </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="H5" t="s">
         <v>57</v>
       </c>
       <c r="J5" t="s">
         <v>58</v>
       </c>
-      <c r="P5" t="s">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="Q5" t="s">
@@ -2545,16 +2564,21 @@
       </c>
     </row>
     <row r="6" spans="1:25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
       </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="K6" t="s">
         <v>69</v>
       </c>
-      <c r="P6" t="s">
+      <c r="O6" s="5"/>
+      <c r="P6" s="5" t="s">
         <v>70</v>
       </c>
       <c r="Q6" t="s">
@@ -2577,13 +2601,18 @@
       </c>
     </row>
     <row r="7" spans="1:25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
-      <c r="P7" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5" t="s">
         <v>70</v>
       </c>
       <c r="Q7" t="s">
@@ -2591,19 +2620,23 @@
       </c>
     </row>
     <row r="8" spans="1:25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="J8" t="s">
         <v>78</v>
       </c>
-      <c r="P8" t="s">
+      <c r="O8" s="5"/>
+      <c r="P8" s="5" t="s">
         <v>79</v>
       </c>
       <c r="Q8" t="s">
@@ -2617,31 +2650,31 @@
       </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>81</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>84</v>
       </c>
       <c r="G9" t="s">
         <v>44</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="5" t="s">
         <v>85</v>
       </c>
       <c r="Q9" t="s">
@@ -2655,18 +2688,20 @@
       </c>
     </row>
     <row r="10" spans="1:25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B10" t="s">
         <v>89</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>91</v>
       </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" t="s">
         <v>44</v>
       </c>
@@ -2676,7 +2711,8 @@
       <c r="J10" t="s">
         <v>92</v>
       </c>
-      <c r="P10" t="s">
+      <c r="O10" s="5"/>
+      <c r="P10" s="5" t="s">
         <v>93</v>
       </c>
       <c r="Q10" t="s">
@@ -2708,15 +2744,18 @@
       </c>
     </row>
     <row r="11" spans="1:25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B11" t="s">
         <v>102</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
       <c r="J11" t="s">
         <v>103</v>
       </c>
@@ -2726,7 +2765,8 @@
       <c r="N11" t="s">
         <v>105</v>
       </c>
-      <c r="P11" t="s">
+      <c r="O11" s="5"/>
+      <c r="P11" s="5" t="s">
         <v>106</v>
       </c>
       <c r="Q11" t="s">
@@ -2752,25 +2792,28 @@
       </c>
     </row>
     <row r="12" spans="1:25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B12" t="s">
         <v>109</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
         <v>91</v>
       </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="H12" t="s">
         <v>111</v>
       </c>
       <c r="L12" t="s">
         <v>112</v>
       </c>
-      <c r="P12" t="s">
+      <c r="O12" s="5"/>
+      <c r="P12" s="5" t="s">
         <v>113</v>
       </c>
       <c r="Q12" t="s">
@@ -2793,16 +2836,20 @@
       </c>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>120</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="P13" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5" t="s">
         <v>122</v>
       </c>
       <c r="Q13" t="s">
@@ -2813,16 +2860,18 @@
       </c>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B14" t="s">
         <v>125</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="5"/>
+      <c r="F14" s="5">
         <v>0</v>
       </c>
       <c r="H14" t="s">
@@ -2837,7 +2886,8 @@
       <c r="L14" t="s">
         <v>130</v>
       </c>
-      <c r="P14" t="s">
+      <c r="O14" s="5"/>
+      <c r="P14" s="5" t="s">
         <v>131</v>
       </c>
       <c r="Q14" t="s">
@@ -2854,19 +2904,23 @@
       </c>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B15" t="s">
         <v>134</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
       <c r="G15" t="s">
         <v>44</v>
       </c>
-      <c r="P15" t="s">
+      <c r="O15" s="5"/>
+      <c r="P15" s="5" t="s">
         <v>135</v>
       </c>
       <c r="Q15" t="s">
@@ -2874,16 +2928,21 @@
       </c>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>137</v>
       </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
       <c r="G16" t="s">
         <v>44</v>
       </c>
-      <c r="P16" t="s">
+      <c r="O16" s="5"/>
+      <c r="P16" s="5" t="s">
         <v>138</v>
       </c>
       <c r="Q16" t="s">
@@ -2894,19 +2953,23 @@
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>140</v>
       </c>
       <c r="B17" t="s">
         <v>141</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
         <v>56</v>
       </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
       <c r="J17" t="s">
         <v>142</v>
       </c>
-      <c r="P17" t="s">
+      <c r="O17" s="5"/>
+      <c r="P17" s="5" t="s">
         <v>143</v>
       </c>
       <c r="Q17" t="s">
@@ -2926,19 +2989,23 @@
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>148</v>
       </c>
       <c r="B18" t="s">
         <v>149</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
         <v>150</v>
       </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
       <c r="G18" t="s">
         <v>44</v>
       </c>
-      <c r="P18" t="s">
+      <c r="O18" s="5"/>
+      <c r="P18" s="5" t="s">
         <v>151</v>
       </c>
       <c r="Q18" t="s">
@@ -2949,22 +3016,25 @@
       </c>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>153</v>
       </c>
       <c r="B19" t="s">
         <v>154</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="s">
         <v>156</v>
       </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
       <c r="G19" t="s">
         <v>157</v>
       </c>
-      <c r="P19" t="s">
+      <c r="O19" s="5"/>
+      <c r="P19" s="5" t="s">
         <v>158</v>
       </c>
       <c r="Q19" t="s">
@@ -2975,15 +3045,18 @@
       </c>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" t="s">
+      <c r="A20" s="5" t="s">
         <v>160</v>
       </c>
       <c r="B20" t="s">
         <v>161</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
         <v>162</v>
       </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
       <c r="G20" t="s">
         <v>163</v>
       </c>
@@ -2996,10 +3069,10 @@
       <c r="L20" t="s">
         <v>166</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="5" t="s">
         <v>168</v>
       </c>
       <c r="Q20" t="s">
@@ -3010,15 +3083,18 @@
       </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B21" t="s">
         <v>172</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
         <v>173</v>
       </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="G21" t="s">
         <v>44</v>
       </c>
@@ -3034,10 +3110,10 @@
       <c r="M21" t="s">
         <v>177</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="5" t="s">
         <v>179</v>
       </c>
       <c r="Q21" t="s">
@@ -3051,15 +3127,18 @@
       </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B22" t="s">
         <v>184</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
         <v>185</v>
       </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
       <c r="G22" t="s">
         <v>44</v>
       </c>
@@ -3072,10 +3151,10 @@
       <c r="L22" t="s">
         <v>187</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="5" t="s">
         <v>179</v>
       </c>
       <c r="Q22" t="s">
@@ -3089,13 +3168,18 @@
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>190</v>
       </c>
       <c r="B23" t="s">
         <v>191</v>
       </c>
-      <c r="P23" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5" t="s">
         <v>192</v>
       </c>
       <c r="Q23" t="s">
@@ -3106,16 +3190,20 @@
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>194</v>
       </c>
       <c r="B24" t="s">
         <v>195</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="P24" t="s">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5" t="s">
         <v>197</v>
       </c>
       <c r="Q24" t="s">
@@ -3129,19 +3217,23 @@
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" t="s">
+      <c r="A25" s="5" t="s">
         <v>199</v>
       </c>
       <c r="B25" t="s">
         <v>200</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
         <v>201</v>
       </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
       <c r="G25" t="s">
         <v>202</v>
       </c>
-      <c r="P25" t="s">
+      <c r="O25" s="5"/>
+      <c r="P25" s="5" t="s">
         <v>203</v>
       </c>
       <c r="Q25" t="s">
@@ -3155,19 +3247,22 @@
       </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26" t="s">
+      <c r="A26" s="5" t="s">
         <v>205</v>
       </c>
       <c r="B26" t="s">
         <v>206</v>
       </c>
-      <c r="E26" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="O26" t="s">
+      <c r="F26" s="5"/>
+      <c r="O26" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="5" t="s">
         <v>208</v>
       </c>
       <c r="Q26" t="s">
@@ -3181,16 +3276,21 @@
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" t="s">
+      <c r="A27" s="5" t="s">
         <v>211</v>
       </c>
       <c r="B27" t="s">
         <v>212</v>
       </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
       <c r="G27" t="s">
         <v>202</v>
       </c>
-      <c r="P27" t="s">
+      <c r="O27" s="5"/>
+      <c r="P27" s="5" t="s">
         <v>213</v>
       </c>
       <c r="Q27" t="s">
@@ -3207,19 +3307,23 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" t="s">
+      <c r="A28" s="5" t="s">
         <v>217</v>
       </c>
       <c r="B28" t="s">
         <v>218</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
         <v>219</v>
       </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
       <c r="G28" t="s">
         <v>202</v>
       </c>
-      <c r="P28" t="s">
+      <c r="O28" s="5"/>
+      <c r="P28" s="5" t="s">
         <v>220</v>
       </c>
       <c r="Q28" t="s">
@@ -3233,19 +3337,20 @@
       </c>
     </row>
     <row r="29" spans="1:22" s="1" customFormat="1">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="6" t="s">
         <v>223</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="6" t="s">
         <v>227</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -3257,10 +3362,10 @@
       <c r="J29" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="O29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="P29" s="6" t="s">
         <v>230</v>
       </c>
       <c r="Q29" s="1" t="s">
@@ -3277,22 +3382,26 @@
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" t="s">
+      <c r="A30" s="5" t="s">
         <v>234</v>
       </c>
       <c r="B30" t="s">
         <v>235</v>
       </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
       <c r="K30" t="s">
         <v>236</v>
       </c>
       <c r="L30" t="s">
         <v>237</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="5" t="s">
         <v>238</v>
       </c>
       <c r="Q30" t="s">
@@ -3306,19 +3415,20 @@
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" t="s">
+      <c r="A31" s="5" t="s">
         <v>242</v>
       </c>
       <c r="B31" t="s">
         <v>243</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="5" t="s">
         <v>246</v>
       </c>
       <c r="G31" t="s">
@@ -3333,10 +3443,10 @@
       <c r="J31" t="s">
         <v>248</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P31" s="5" t="s">
         <v>251</v>
       </c>
       <c r="Q31" t="s">
@@ -3350,19 +3460,20 @@
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
         <v>255</v>
       </c>
       <c r="B32" t="s">
         <v>256</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="5" t="s">
         <v>258</v>
       </c>
       <c r="G32" t="s">
@@ -3377,7 +3488,8 @@
       <c r="J32" t="s">
         <v>261</v>
       </c>
-      <c r="P32" t="s">
+      <c r="O32" s="5"/>
+      <c r="P32" s="5" t="s">
         <v>251</v>
       </c>
       <c r="Q32" t="s">
@@ -3391,15 +3503,18 @@
       </c>
     </row>
     <row r="33" spans="1:23">
-      <c r="A33" t="s">
+      <c r="A33" s="5" t="s">
         <v>264</v>
       </c>
       <c r="B33" t="s">
         <v>265</v>
       </c>
-      <c r="E33" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
         <v>266</v>
       </c>
+      <c r="F33" s="5"/>
       <c r="G33" t="s">
         <v>267</v>
       </c>
@@ -3412,7 +3527,8 @@
       <c r="L33" t="s">
         <v>270</v>
       </c>
-      <c r="P33" t="s">
+      <c r="O33" s="5"/>
+      <c r="P33" s="5" t="s">
         <v>271</v>
       </c>
       <c r="Q33" t="s">
@@ -3432,19 +3548,20 @@
       </c>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" t="s">
+      <c r="A34" s="5" t="s">
         <v>276</v>
       </c>
       <c r="B34" t="s">
         <v>277</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="E34" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="5" t="s">
         <v>280</v>
       </c>
       <c r="G34" t="s">
@@ -3456,7 +3573,8 @@
       <c r="I34" t="s">
         <v>282</v>
       </c>
-      <c r="P34" t="s">
+      <c r="O34" s="5"/>
+      <c r="P34" s="5" t="s">
         <v>271</v>
       </c>
       <c r="Q34" t="s">
@@ -3467,15 +3585,18 @@
       </c>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" t="s">
+      <c r="A35" s="5" t="s">
         <v>284</v>
       </c>
       <c r="B35" t="s">
         <v>285</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="5" t="s">
         <v>286</v>
       </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
       <c r="H35" t="s">
         <v>287</v>
       </c>
@@ -3485,7 +3606,8 @@
       <c r="J35" t="s">
         <v>289</v>
       </c>
-      <c r="P35" t="s">
+      <c r="O35" s="5"/>
+      <c r="P35" s="5" t="s">
         <v>290</v>
       </c>
       <c r="Q35" t="s">
@@ -3508,12 +3630,16 @@
       </c>
     </row>
     <row r="36" spans="1:23">
-      <c r="A36" t="s">
+      <c r="A36" s="5" t="s">
         <v>296</v>
       </c>
       <c r="B36" t="s">
         <v>297</v>
       </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
       <c r="H36" t="s">
         <v>298</v>
       </c>
@@ -3523,7 +3649,8 @@
       <c r="J36" t="s">
         <v>289</v>
       </c>
-      <c r="P36" t="s">
+      <c r="O36" s="5"/>
+      <c r="P36" s="5" t="s">
         <v>299</v>
       </c>
       <c r="Q36" t="s">
@@ -3546,19 +3673,20 @@
       </c>
     </row>
     <row r="37" spans="1:23">
-      <c r="A37" t="s">
+      <c r="A37" s="5" t="s">
         <v>302</v>
       </c>
       <c r="B37" t="s">
         <v>303</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="5">
         <v>1964</v>
       </c>
       <c r="G37" t="s">
@@ -3585,7 +3713,8 @@
       <c r="N37" t="s">
         <v>287</v>
       </c>
-      <c r="P37" t="s">
+      <c r="O37" s="5"/>
+      <c r="P37" s="5" t="s">
         <v>299</v>
       </c>
       <c r="Q37" t="s">
@@ -3596,13 +3725,18 @@
       </c>
     </row>
     <row r="38" spans="1:23">
-      <c r="A38" t="s">
+      <c r="A38" s="5" t="s">
         <v>313</v>
       </c>
       <c r="B38" t="s">
         <v>314</v>
       </c>
-      <c r="P38" t="s">
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5" t="s">
         <v>315</v>
       </c>
       <c r="Q38" t="s">
@@ -3613,22 +3747,22 @@
       </c>
     </row>
     <row r="39" spans="1:23">
-      <c r="A39" t="s">
+      <c r="A39" s="5" t="s">
         <v>317</v>
       </c>
       <c r="B39" t="s">
         <v>318</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="5" t="s">
         <v>322</v>
       </c>
       <c r="G39" t="s">
@@ -3640,7 +3774,8 @@
       <c r="J39" t="s">
         <v>324</v>
       </c>
-      <c r="P39" t="s">
+      <c r="O39" s="5"/>
+      <c r="P39" s="5" t="s">
         <v>325</v>
       </c>
       <c r="Q39" t="s">
@@ -3654,22 +3789,22 @@
       </c>
     </row>
     <row r="40" spans="1:23">
-      <c r="A40" t="s">
+      <c r="A40" s="5" t="s">
         <v>328</v>
       </c>
       <c r="B40" t="s">
         <v>329</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="5" t="s">
         <v>333</v>
       </c>
       <c r="G40" t="s">
@@ -3681,7 +3816,8 @@
       <c r="J40" t="s">
         <v>336</v>
       </c>
-      <c r="P40" t="s">
+      <c r="O40" s="5"/>
+      <c r="P40" s="5" t="s">
         <v>337</v>
       </c>
       <c r="Q40" t="s">
@@ -3689,16 +3825,18 @@
       </c>
     </row>
     <row r="41" spans="1:23">
-      <c r="A41" t="s">
+      <c r="A41" s="5" t="s">
         <v>338</v>
       </c>
       <c r="B41" t="s">
         <v>339</v>
       </c>
-      <c r="E41" t="s">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="5" t="s">
         <v>340</v>
       </c>
       <c r="G41" t="s">
@@ -3710,7 +3848,8 @@
       <c r="I41" t="s">
         <v>342</v>
       </c>
-      <c r="P41" t="s">
+      <c r="O41" s="5"/>
+      <c r="P41" s="5" t="s">
         <v>337</v>
       </c>
       <c r="Q41" t="s">
@@ -3718,22 +3857,25 @@
       </c>
     </row>
     <row r="42" spans="1:23">
-      <c r="A42" t="s">
+      <c r="A42" s="5" t="s">
         <v>343</v>
       </c>
       <c r="B42" t="s">
         <v>344</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="5" t="s">
         <v>346</v>
       </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
       <c r="G42" t="s">
         <v>334</v>
       </c>
-      <c r="P42" t="s">
+      <c r="O42" s="5"/>
+      <c r="P42" s="5" t="s">
         <v>347</v>
       </c>
       <c r="Q42" t="s">
@@ -3741,13 +3883,18 @@
       </c>
     </row>
     <row r="43" spans="1:23">
-      <c r="A43" t="s">
+      <c r="A43" s="5" t="s">
         <v>348</v>
       </c>
       <c r="B43" t="s">
         <v>349</v>
       </c>
-      <c r="P43" t="s">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5" t="s">
         <v>350</v>
       </c>
       <c r="Q43" t="s">
@@ -3755,18 +3902,20 @@
       </c>
     </row>
     <row r="44" spans="1:23">
-      <c r="A44" t="s">
+      <c r="A44" s="5" t="s">
         <v>351</v>
       </c>
       <c r="B44" t="s">
         <v>352</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="5" t="s">
         <v>245</v>
       </c>
+      <c r="F44" s="5"/>
       <c r="G44" t="s">
         <v>306</v>
       </c>
@@ -3779,7 +3928,8 @@
       <c r="J44" t="s">
         <v>356</v>
       </c>
-      <c r="P44" t="s">
+      <c r="O44" s="5"/>
+      <c r="P44" s="5" t="s">
         <v>315</v>
       </c>
       <c r="Q44" t="s">
@@ -3787,22 +3937,26 @@
       </c>
     </row>
     <row r="45" spans="1:23">
-      <c r="A45" t="s">
+      <c r="A45" s="5" t="s">
         <v>357</v>
       </c>
       <c r="B45" t="s">
         <v>358</v>
       </c>
-      <c r="D45" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
         <v>359</v>
       </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
       <c r="G45" t="s">
         <v>360</v>
       </c>
       <c r="J45" t="s">
         <v>361</v>
       </c>
-      <c r="P45" t="s">
+      <c r="O45" s="5"/>
+      <c r="P45" s="5" t="s">
         <v>347</v>
       </c>
       <c r="Q45" t="s">
@@ -3810,25 +3964,28 @@
       </c>
     </row>
     <row r="46" spans="1:23">
-      <c r="A46" t="s">
+      <c r="A46" s="5" t="s">
         <v>362</v>
       </c>
       <c r="B46" t="s">
         <v>363</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="5" t="s">
         <v>245</v>
       </c>
+      <c r="F46" s="5"/>
       <c r="G46" t="s">
         <v>245</v>
       </c>
       <c r="J46" t="s">
         <v>269</v>
       </c>
-      <c r="P46" t="s">
+      <c r="O46" s="5"/>
+      <c r="P46" s="5" t="s">
         <v>365</v>
       </c>
       <c r="Q46" t="s">
@@ -3839,22 +3996,26 @@
       </c>
     </row>
     <row r="47" spans="1:23">
-      <c r="A47" t="s">
+      <c r="A47" s="5" t="s">
         <v>367</v>
       </c>
       <c r="B47" t="s">
         <v>368</v>
       </c>
-      <c r="E47" t="s">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
         <v>369</v>
       </c>
+      <c r="F47" s="5"/>
       <c r="H47" t="s">
         <v>370</v>
       </c>
       <c r="I47" t="s">
         <v>371</v>
       </c>
-      <c r="P47" t="s">
+      <c r="O47" s="5"/>
+      <c r="P47" s="5" t="s">
         <v>350</v>
       </c>
       <c r="Q47" t="s">
@@ -3862,15 +4023,18 @@
       </c>
     </row>
     <row r="48" spans="1:23">
-      <c r="A48" t="s">
+      <c r="A48" s="5" t="s">
         <v>372</v>
       </c>
       <c r="B48" t="s">
         <v>373</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5" t="s">
         <v>374</v>
       </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
       <c r="G48" t="s">
         <v>375</v>
       </c>
@@ -3883,7 +4047,8 @@
       <c r="J48" t="s">
         <v>378</v>
       </c>
-      <c r="P48" t="s">
+      <c r="O48" s="5"/>
+      <c r="P48" s="5" t="s">
         <v>379</v>
       </c>
       <c r="Q48" t="s">
@@ -3903,19 +4068,22 @@
       </c>
     </row>
     <row r="49" spans="1:26">
-      <c r="A49" t="s">
+      <c r="A49" s="5" t="s">
         <v>384</v>
       </c>
       <c r="B49" t="s">
         <v>385</v>
       </c>
-      <c r="E49" t="s">
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="5">
         <v>1971</v>
       </c>
-      <c r="P49" t="s">
+      <c r="O49" s="5"/>
+      <c r="P49" s="5" t="s">
         <v>387</v>
       </c>
       <c r="Q49" t="s">
@@ -3926,15 +4094,18 @@
       </c>
     </row>
     <row r="50" spans="1:26">
-      <c r="A50" t="s">
+      <c r="A50" s="5" t="s">
         <v>389</v>
       </c>
       <c r="B50" t="s">
         <v>390</v>
       </c>
-      <c r="D50">
+      <c r="C50" s="5"/>
+      <c r="D50" s="5">
         <v>1940</v>
       </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
       <c r="K50" t="s">
         <v>391</v>
       </c>
@@ -3947,7 +4118,8 @@
       <c r="N50" t="s">
         <v>394</v>
       </c>
-      <c r="P50" t="s">
+      <c r="O50" s="5"/>
+      <c r="P50" s="5" t="s">
         <v>395</v>
       </c>
       <c r="Q50" t="s">
@@ -3955,15 +4127,18 @@
       </c>
     </row>
     <row r="51" spans="1:26">
-      <c r="A51" t="s">
+      <c r="A51" s="5" t="s">
         <v>396</v>
       </c>
       <c r="B51" t="s">
         <v>391</v>
       </c>
-      <c r="D51" t="s">
+      <c r="C51" s="5"/>
+      <c r="D51" s="5" t="s">
         <v>397</v>
       </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
       <c r="G51" t="s">
         <v>398</v>
       </c>
@@ -3973,7 +4148,8 @@
       <c r="I51" t="s">
         <v>400</v>
       </c>
-      <c r="P51" t="s">
+      <c r="O51" s="5"/>
+      <c r="P51" s="5" t="s">
         <v>395</v>
       </c>
       <c r="Q51" t="s">
@@ -4008,19 +4184,20 @@
       </c>
     </row>
     <row r="52" spans="1:26">
-      <c r="A52" t="s">
+      <c r="A52" s="5" t="s">
         <v>410</v>
       </c>
       <c r="B52" t="s">
         <v>411</v>
       </c>
-      <c r="D52">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5">
         <v>1958</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="5">
         <v>1967</v>
       </c>
       <c r="G52" t="s">
@@ -4032,7 +4209,8 @@
       <c r="I52" t="s">
         <v>414</v>
       </c>
-      <c r="P52" t="s">
+      <c r="O52" s="5"/>
+      <c r="P52" s="5" t="s">
         <v>415</v>
       </c>
       <c r="Q52" t="s">
@@ -4043,21 +4221,22 @@
       </c>
     </row>
     <row r="53" spans="1:26">
-      <c r="A53" t="s">
+      <c r="A53" s="5" t="s">
         <v>417</v>
       </c>
       <c r="B53" t="s">
         <v>418</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="5" t="s">
         <v>421</v>
       </c>
+      <c r="F53" s="5"/>
       <c r="G53" t="s">
         <v>422</v>
       </c>
@@ -4070,7 +4249,8 @@
       <c r="J53" t="s">
         <v>424</v>
       </c>
-      <c r="P53" t="s">
+      <c r="O53" s="5"/>
+      <c r="P53" s="5" t="s">
         <v>425</v>
       </c>
       <c r="Q53" t="s">
@@ -4078,15 +4258,18 @@
       </c>
     </row>
     <row r="54" spans="1:26">
-      <c r="A54" t="s">
+      <c r="A54" s="5" t="s">
         <v>426</v>
       </c>
       <c r="B54" t="s">
         <v>427</v>
       </c>
-      <c r="D54">
+      <c r="C54" s="5"/>
+      <c r="D54" s="5">
         <v>1947</v>
       </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
       <c r="G54" t="s">
         <v>428</v>
       </c>
@@ -4096,7 +4279,8 @@
       <c r="J54" t="s">
         <v>429</v>
       </c>
-      <c r="P54" t="s">
+      <c r="O54" s="5"/>
+      <c r="P54" s="5" t="s">
         <v>430</v>
       </c>
       <c r="Q54" t="s">
@@ -4104,15 +4288,18 @@
       </c>
     </row>
     <row r="55" spans="1:26">
-      <c r="A55" t="s">
+      <c r="A55" s="5" t="s">
         <v>431</v>
       </c>
       <c r="B55" t="s">
         <v>432</v>
       </c>
-      <c r="D55" t="s">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5" t="s">
         <v>433</v>
       </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="G55" t="s">
         <v>434</v>
       </c>
@@ -4122,7 +4309,8 @@
       <c r="J55" t="s">
         <v>436</v>
       </c>
-      <c r="P55" t="s">
+      <c r="O55" s="5"/>
+      <c r="P55" s="5" t="s">
         <v>437</v>
       </c>
       <c r="Q55" t="s">
@@ -4130,15 +4318,18 @@
       </c>
     </row>
     <row r="56" spans="1:26">
-      <c r="A56" t="s">
+      <c r="A56" s="5" t="s">
         <v>438</v>
       </c>
       <c r="B56" t="s">
         <v>439</v>
       </c>
-      <c r="D56" t="s">
+      <c r="C56" s="5"/>
+      <c r="D56" s="5" t="s">
         <v>440</v>
       </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
       <c r="G56" t="s">
         <v>441</v>
       </c>
@@ -4151,7 +4342,8 @@
       <c r="J56" t="s">
         <v>442</v>
       </c>
-      <c r="P56" t="s">
+      <c r="O56" s="5"/>
+      <c r="P56" s="5" t="s">
         <v>437</v>
       </c>
       <c r="Q56" t="s">
@@ -4159,15 +4351,18 @@
       </c>
     </row>
     <row r="57" spans="1:26">
-      <c r="A57" t="s">
+      <c r="A57" s="5" t="s">
         <v>444</v>
       </c>
       <c r="B57" t="s">
         <v>445</v>
       </c>
-      <c r="D57" t="s">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5" t="s">
         <v>446</v>
       </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
       <c r="G57" t="s">
         <v>447</v>
       </c>
@@ -4180,7 +4375,8 @@
       <c r="J57" t="s">
         <v>442</v>
       </c>
-      <c r="P57" t="s">
+      <c r="O57" s="5"/>
+      <c r="P57" s="5" t="s">
         <v>437</v>
       </c>
       <c r="Q57" t="s">
@@ -4188,22 +4384,26 @@
       </c>
     </row>
     <row r="58" spans="1:26">
-      <c r="A58" t="s">
+      <c r="A58" s="5" t="s">
         <v>448</v>
       </c>
       <c r="B58" t="s">
         <v>449</v>
       </c>
-      <c r="E58" t="s">
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="F58" s="5"/>
       <c r="H58" t="s">
         <v>370</v>
       </c>
       <c r="I58" t="s">
         <v>371</v>
       </c>
-      <c r="P58" t="s">
+      <c r="O58" s="5"/>
+      <c r="P58" s="5" t="s">
         <v>450</v>
       </c>
       <c r="Q58" t="s">
@@ -4211,13 +4411,18 @@
       </c>
     </row>
     <row r="59" spans="1:26">
-      <c r="A59" t="s">
+      <c r="A59" s="5" t="s">
         <v>451</v>
       </c>
       <c r="B59" t="s">
         <v>452</v>
       </c>
-      <c r="P59" t="s">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5" t="s">
         <v>290</v>
       </c>
       <c r="Q59" t="s">
@@ -4228,21 +4433,22 @@
       </c>
     </row>
     <row r="60" spans="1:26">
-      <c r="A60" t="s">
+      <c r="A60" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B60" t="s">
         <v>455</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="5" t="s">
         <v>245</v>
       </c>
+      <c r="F60" s="5"/>
       <c r="H60" t="s">
         <v>458</v>
       </c>
@@ -4252,7 +4458,8 @@
       <c r="J60" t="s">
         <v>460</v>
       </c>
-      <c r="P60" t="s">
+      <c r="O60" s="5"/>
+      <c r="P60" s="5" t="s">
         <v>461</v>
       </c>
       <c r="Q60" t="s">
@@ -4260,18 +4467,20 @@
       </c>
     </row>
     <row r="61" spans="1:26">
-      <c r="A61" t="s">
+      <c r="A61" s="5" t="s">
         <v>462</v>
       </c>
       <c r="B61" t="s">
         <v>463</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="5" t="s">
         <v>465</v>
       </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
       <c r="G61" t="s">
         <v>466</v>
       </c>
@@ -4284,20 +4493,25 @@
       <c r="J61" t="s">
         <v>467</v>
       </c>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
       <c r="Q61" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:26">
-      <c r="A62" t="s">
+      <c r="A62" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B62" t="s">
         <v>469</v>
       </c>
-      <c r="D62" t="s">
+      <c r="C62" s="5"/>
+      <c r="D62" s="5" t="s">
         <v>470</v>
       </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
       <c r="G62" t="s">
         <v>471</v>
       </c>
@@ -4310,7 +4524,8 @@
       <c r="M62" t="s">
         <v>474</v>
       </c>
-      <c r="P62" t="s">
+      <c r="O62" s="5"/>
+      <c r="P62" s="5" t="s">
         <v>475</v>
       </c>
       <c r="Q62" t="s">
@@ -4321,16 +4536,17 @@
       </c>
     </row>
     <row r="63" spans="1:26">
-      <c r="A63" t="s">
+      <c r="A63" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="D63" t="s">
+      <c r="C63" s="5"/>
+      <c r="D63" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="5" t="s">
         <v>480</v>
       </c>
       <c r="G63" t="s">
@@ -4342,10 +4558,10 @@
       <c r="L63" t="s">
         <v>481</v>
       </c>
-      <c r="O63" t="s">
+      <c r="O63" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P63" s="5" t="s">
         <v>483</v>
       </c>
       <c r="Q63" t="s">
@@ -4353,15 +4569,18 @@
       </c>
     </row>
     <row r="64" spans="1:26">
-      <c r="A64" t="s">
+      <c r="A64" s="5" t="s">
         <v>484</v>
       </c>
       <c r="B64" t="s">
         <v>485</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" s="5"/>
+      <c r="D64" s="5" t="s">
         <v>121</v>
       </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
       <c r="H64" t="s">
         <v>486</v>
       </c>
@@ -4374,7 +4593,8 @@
       <c r="L64" t="s">
         <v>489</v>
       </c>
-      <c r="P64" t="s">
+      <c r="O64" s="5"/>
+      <c r="P64" s="5" t="s">
         <v>490</v>
       </c>
       <c r="Q64" t="s">
@@ -4382,19 +4602,24 @@
       </c>
     </row>
     <row r="65" spans="1:18">
-      <c r="A65" t="s">
+      <c r="A65" s="5" t="s">
         <v>491</v>
       </c>
       <c r="B65" t="s">
         <v>492</v>
       </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
       <c r="H65" t="s">
         <v>165</v>
       </c>
       <c r="L65" t="s">
         <v>493</v>
       </c>
-      <c r="P65" t="s">
+      <c r="O65" s="5"/>
+      <c r="P65" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q65" t="s">
@@ -4405,19 +4630,23 @@
       </c>
     </row>
     <row r="66" spans="1:18">
-      <c r="A66" t="s">
+      <c r="A66" s="5" t="s">
         <v>496</v>
       </c>
       <c r="B66" t="s">
         <v>497</v>
       </c>
-      <c r="D66" t="s">
+      <c r="C66" s="5"/>
+      <c r="D66" s="5" t="s">
         <v>498</v>
       </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
       <c r="H66" t="s">
         <v>165</v>
       </c>
-      <c r="P66" t="s">
+      <c r="O66" s="5"/>
+      <c r="P66" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q66" t="s">
@@ -4428,22 +4657,25 @@
       </c>
     </row>
     <row r="67" spans="1:18">
-      <c r="A67" t="s">
+      <c r="A67" s="5" t="s">
         <v>499</v>
       </c>
       <c r="B67" t="s">
         <v>500</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="5" t="s">
         <v>501</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="D67" s="5"/>
+      <c r="E67" s="7" t="s">
         <v>502</v>
       </c>
+      <c r="F67" s="5"/>
       <c r="H67" t="s">
         <v>165</v>
       </c>
-      <c r="P67" t="s">
+      <c r="O67" s="5"/>
+      <c r="P67" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q67" t="s">
@@ -4454,16 +4686,21 @@
       </c>
     </row>
     <row r="68" spans="1:18">
-      <c r="A68" t="s">
+      <c r="A68" s="5" t="s">
         <v>503</v>
       </c>
       <c r="B68" t="s">
         <v>504</v>
       </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
       <c r="H68" t="s">
         <v>165</v>
       </c>
-      <c r="P68" t="s">
+      <c r="O68" s="5"/>
+      <c r="P68" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q68" t="s">
@@ -4474,16 +4711,21 @@
       </c>
     </row>
     <row r="69" spans="1:18">
-      <c r="A69" t="s">
+      <c r="A69" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>506</v>
       </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
       <c r="H69" t="s">
         <v>165</v>
       </c>
-      <c r="P69" t="s">
+      <c r="O69" s="5"/>
+      <c r="P69" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q69" t="s">
@@ -4494,22 +4736,27 @@
       </c>
     </row>
     <row r="70" spans="1:18">
-      <c r="A70" t="s">
+      <c r="A70" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>508</v>
       </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
       <c r="H70" t="s">
         <v>165</v>
       </c>
-      <c r="K70" s="5" t="s">
+      <c r="K70" s="4" t="s">
         <v>509</v>
       </c>
       <c r="L70" t="s">
         <v>510</v>
       </c>
-      <c r="P70" t="s">
+      <c r="O70" s="5"/>
+      <c r="P70" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q70" t="s">
@@ -4520,16 +4767,21 @@
       </c>
     </row>
     <row r="71" spans="1:18">
-      <c r="A71" t="s">
+      <c r="A71" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>512</v>
       </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
       <c r="H71" t="s">
         <v>165</v>
       </c>
-      <c r="P71" t="s">
+      <c r="O71" s="5"/>
+      <c r="P71" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q71" t="s">
@@ -4540,16 +4792,21 @@
       </c>
     </row>
     <row r="72" spans="1:18">
-      <c r="A72" t="s">
+      <c r="A72" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>514</v>
       </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
       <c r="H72" t="s">
         <v>165</v>
       </c>
-      <c r="P72" t="s">
+      <c r="O72" s="5"/>
+      <c r="P72" s="5" t="s">
         <v>515</v>
       </c>
       <c r="Q72" t="s">
@@ -4560,19 +4817,20 @@
       </c>
     </row>
     <row r="73" spans="1:18">
-      <c r="A73" t="s">
+      <c r="A73" s="5" t="s">
         <v>516</v>
       </c>
       <c r="B73" t="s">
         <v>517</v>
       </c>
-      <c r="D73" t="s">
+      <c r="C73" s="5"/>
+      <c r="D73" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="5" t="s">
         <v>518</v>
       </c>
       <c r="G73" t="s">
@@ -4593,7 +4851,8 @@
       <c r="N73" t="s">
         <v>522</v>
       </c>
-      <c r="P73" t="s">
+      <c r="O73" s="5"/>
+      <c r="P73" s="5" t="s">
         <v>494</v>
       </c>
       <c r="Q73" t="s">
@@ -4601,15 +4860,18 @@
       </c>
     </row>
     <row r="74" spans="1:18">
-      <c r="A74" t="s">
+      <c r="A74" s="5" t="s">
         <v>523</v>
       </c>
       <c r="B74" t="s">
         <v>525</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C74" s="5"/>
+      <c r="D74" s="5" t="s">
         <v>150</v>
       </c>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
       <c r="G74" t="s">
         <v>360</v>
       </c>
@@ -4622,7 +4884,8 @@
       <c r="N74" t="s">
         <v>529</v>
       </c>
-      <c r="P74" t="s">
+      <c r="O74" s="5"/>
+      <c r="P74" s="5" t="s">
         <v>524</v>
       </c>
       <c r="Q74" t="s">
@@ -4633,16 +4896,17 @@
       </c>
     </row>
     <row r="75" spans="1:18">
-      <c r="A75" t="s">
+      <c r="A75" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="D75" t="s">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="5" t="s">
         <v>535</v>
       </c>
       <c r="G75" t="s">
@@ -4663,7 +4927,8 @@
       <c r="N75" t="s">
         <v>532</v>
       </c>
-      <c r="P75" t="s">
+      <c r="O75" s="5"/>
+      <c r="P75" s="5" t="s">
         <v>524</v>
       </c>
       <c r="Q75" t="s">

</xml_diff>